<commit_message>
Adde my comments to review table
</commit_message>
<xml_diff>
--- a/Submission/Re-submission/reviews_table.xlsx
+++ b/Submission/Re-submission/reviews_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liviosilva-muller/Documents/GitHub/amazondef/Submission/Re-submission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henriquesposito/Documents/GitHub/amazondef/Submission/Re-submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D00839-41DB-B24A-B30F-352580C1C841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A38B74-5104-4F46-9BE8-E5DF0A803716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" xr2:uid="{6CFD92DF-9600-EC4C-BBE6-9FD001CE7D96}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" activeTab="5" xr2:uid="{6CFD92DF-9600-EC4C-BBE6-9FD001CE7D96}"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="105">
   <si>
     <t>Comment by reviewer</t>
   </si>
@@ -297,6 +297,69 @@
   </si>
   <si>
     <t>more descriptive, similar to what is 4.1 now.</t>
+  </si>
+  <si>
+    <t>Mention this as this might be both puzzling and expected...</t>
+  </si>
+  <si>
+    <t>Comments HS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't agree but we need to state further that thius comes not only from the environment but also from the economic integration construction. </t>
+  </si>
+  <si>
+    <t>We can, intead of the models, add a similar for within Amazonian states, amazonian countries, non-Amazonian states, and other countries. As we had before. We then move models used to construct these to appendix, as we do with figure 6.</t>
+  </si>
+  <si>
+    <t>The implementation of the above should solve this issue as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe we can build somerthing like problem construction does not look much into setings while 2 level game overlooks about audiences… therefore we theorize this as a multi-level game where what audiences within states, regions, nations, and internationally want to hear (or what politicians expect matters for them) shapes sociocultural problem-constructions; and this is what we should about the Amazon. </t>
+  </si>
+  <si>
+    <t>BTW, I agree here, as I told you before, this is not a standard use of this in IR, though I do not think it is a big issue since we define it at the very top. However, I would say, just to avoid confusion, I would prefer if we can go without transationalism and just connect beter problem construction with the multi level game…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we add other Amazonian countries back into the analysis this also become part fo our concluding remarks = understand this in comparative ways in important to undertand the </t>
+  </si>
+  <si>
+    <t>Remove interest group in favor of international audiences (outside of Amazonian countries).</t>
+  </si>
+  <si>
+    <t>Change to general events that gathered national and international attention.</t>
+  </si>
+  <si>
+    <t>I amnot sure here either, but this might be a way of better closing the paper.</t>
+  </si>
+  <si>
+    <t>We need to get rid off what is not necessary and expand on what is, in my opinion. We do not need chosen vs. Pressing, perhaps only Bacci - on culture and constructions. Also, can we get rid of transnationalism and construct the thin-theory with Bacci + Putnan? This is also a matter of levels, we discuss/theorize/measure discourse but really talk/imply about outcomes/consequences, a thin-line we might need to better walk and justify at the setup and wrap at the conclusion (i.e. in conclusion, this helps us think about how discourse, policy, and outcomes for policy issues interact; whereas problem contructions in discourses might be a better unit of anilysis to study multi-faceted and multi-level policy issues to capture the various, and often paradoxal, policy outcomes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to talk back to literature in the analysis, as we had discussed previously. Once regions is brought back to analysis modelling, we can claim to somewhat better test mechanisms. Also, not a two level but a multi level. Finally, should we bring ideology as a control in the models? I am not sure we should, but if we don't we might always get this question (i.e. what about ideology?). </t>
+  </si>
+  <si>
+    <t>We might be able to extract information on venue, but I am not sure we should. We can compare models with distance to multinomial models by region and with IOs...</t>
+  </si>
+  <si>
+    <t>A different paper in my opinion, but perhapes we can use this in conclusion as a research avenue?</t>
+  </si>
+  <si>
+    <t>Let's clarify this but, in my opinion, we move all regression models to appendix and keep only figures. Because it is an unbalanced panel, should we use pooled OLS with time effects? Easy to justify. Otherwise, we might want to focus the effects on presidents rather than time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great, exactla what we had discussed already!!! We need to move past talking about the Amazon as an issue of environemntal policy! This is one of our great contributions and a way to keep the literature trend troughout (i.e. literature often focus on environemntal policy and aspects, but forgets that the amazon is a bio-socio-political policy object. </t>
+  </si>
+  <si>
+    <t>Again, a good point to bring at the conclusion, as a reserach avenue, alongside the google trends!</t>
+  </si>
+  <si>
+    <t>I know a bit about this literature and I am not sure this is pertinent unless we want to make an argument about why sovereigty increases after 2010? Expectations would be that sovereigty might increase outside or something… In reality, in this case, presidents go (or should go) fundraising for the Amazon internationally so they might just focus on what "fundin" audiences want to hear or are looking for justifications for.</t>
+  </si>
+  <si>
+    <t>Not sure I agree we need transnationalism…</t>
+  </si>
+  <si>
+    <t>I would keep the current structure, move models to appendix and add a visualization of the levels similar to the ones we have for distance…</t>
   </si>
 </sst>
 </file>
@@ -412,10 +475,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -737,9 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1733E3A-D6DE-EF46-8A36-10EAAE072C0D}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,9 +812,10 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,8 +831,11 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F1" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -784,8 +851,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -801,8 +871,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -818,8 +891,11 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
@@ -835,8 +911,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -852,8 +931,11 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
@@ -863,8 +945,11 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
@@ -877,8 +962,11 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>29</v>
       </c>
@@ -894,8 +982,11 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -908,8 +999,11 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -922,8 +1016,11 @@
       <c r="E11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="289" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -939,8 +1036,11 @@
       <c r="E12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
@@ -953,8 +1053,11 @@
       <c r="D13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -970,8 +1073,11 @@
       <c r="E14" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>22</v>
       </c>
@@ -984,8 +1090,11 @@
       <c r="E15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>32</v>
       </c>
@@ -1001,8 +1110,11 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>41</v>
       </c>
@@ -1012,9 +1124,11 @@
       <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="F17" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -1026,6 +1140,9 @@
       </c>
       <c r="D18" t="s">
         <v>9</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -1044,7 +1161,9 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E17" xr:uid="{F1733E3A-D6DE-EF46-8A36-10EAAE072C0D}"/>
@@ -1056,7 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762D34F-F6EA-8643-A46B-D56BEEEE0334}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -1561,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03468F27-AFFF-574F-A20A-65B416C5AE94}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,7 +1693,7 @@
     <col min="4" max="4" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1588,7 +1707,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1597,7 +1716,7 @@
       </c>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:5" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -1608,7 +1727,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -1618,12 +1737,12 @@
       <c r="C4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -1633,10 +1752,13 @@
       <c r="C5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>3</v>
       </c>
@@ -1645,7 +1767,7 @@
       </c>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3.1</v>
       </c>
@@ -1660,7 +1782,7 @@
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3.2</v>
       </c>
@@ -1673,7 +1795,7 @@
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:5" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3.3</v>
       </c>
@@ -1686,7 +1808,7 @@
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>4</v>
       </c>
@@ -1695,7 +1817,7 @@
       </c>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4.0999999999999996</v>
       </c>
@@ -1705,12 +1827,12 @@
       <c r="C11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4.2</v>
       </c>
@@ -1720,10 +1842,10 @@
       <c r="C12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>69</v>
       </c>
@@ -1733,10 +1855,13 @@
       <c r="C13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>71</v>
       </c>
@@ -1746,10 +1871,10 @@
       <c r="C14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>5</v>
       </c>

</xml_diff>